<commit_message>
add substitute part info for a few caps that are no longer available
</commit_message>
<xml_diff>
--- a/Gen1/Assembly/BOM_PSA.xlsx
+++ b/Gen1/Assembly/BOM_PSA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakareka\Documents\GitHub\PRiME\Gen1\Assembly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakareka\Documents\GitHub\PRiME-Gen1\Gen1\Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BF0D20-09C7-4DB5-9260-5D40B13C1737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23175" windowHeight="9615"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PSA" sheetId="2" r:id="rId1"/>
@@ -30,8 +31,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="ADCModule1" type="6" refreshedVersion="5" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="ADCModule1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\kakareka\projects\PRiME\notes\Gen1\BOM\ADCModule.csv" semicolon="1">
       <textFields count="9">
         <textField/>
@@ -46,7 +47,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="PowerModule1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="PowerModule1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\kakareka\projects\PRiME\notes\Gen1\BOM\PowerModule.csv" semicolon="1">
       <textFields count="8">
         <textField/>
@@ -60,7 +61,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="PRiME-MB1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="PRiME-MB1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\kakareka\projects\PRiME\notes\Gen1\BOM\PRiME-MB.csv" semicolon="1">
       <textFields count="11">
         <textField/>
@@ -77,7 +78,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="PWMAttenuation" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="PWMAttenuation" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="1250" sourceFile="C:\Users\kakareka\projects\PRiME\notes\Gen1\BOM\PWMAttenuation.csv" semicolon="1">
       <textFields count="8">
         <textField/>
@@ -95,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="326">
   <si>
     <t>CC2300 battery charger</t>
   </si>
@@ -1067,12 +1068,18 @@
   </si>
   <si>
     <t>see BOM listed below</t>
+  </si>
+  <si>
+    <t>Substitute: EMF212B7105KGHT</t>
+  </si>
+  <si>
+    <t>Substitute: EMF212B7225KGHT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1187,7 +1194,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1204,19 +1211,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PRiME-MB" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="PowerModule" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PowerModule" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ADCModule" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ADCModule" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="PWMAttenuation" connectionId="4" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PWMAttenuation" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="PRiME-MB" connectionId="3" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1515,26 +1522,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:G13"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.26953125" style="2" customWidth="1"/>
     <col min="6" max="6" width="33" style="1" customWidth="1"/>
-    <col min="7" max="7" width="62.42578125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="62.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="58" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1545,7 +1553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1556,7 +1564,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1567,7 +1575,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1578,7 +1586,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1589,7 +1597,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1600,7 +1608,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1611,7 +1619,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1622,7 +1630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1633,7 +1641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1644,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1653,12 +1661,12 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1679,7 +1687,7 @@
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -1702,7 +1710,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1725,7 +1733,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -1748,7 +1756,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -1771,7 +1779,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>6</v>
       </c>
@@ -1794,7 +1802,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -1817,7 +1825,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -1840,7 +1848,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1863,7 +1871,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -1886,7 +1894,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -1909,7 +1917,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -1932,7 +1940,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1941,12 +1949,12 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B26" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>13</v>
       </c>
@@ -1969,7 +1977,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="174" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>48</v>
       </c>
@@ -1992,7 +2000,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>2</v>
       </c>
@@ -2015,7 +2023,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>6</v>
       </c>
@@ -2038,7 +2046,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>6</v>
       </c>
@@ -2061,7 +2069,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>6</v>
       </c>
@@ -2084,7 +2092,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>6</v>
       </c>
@@ -2107,7 +2115,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>6</v>
       </c>
@@ -2130,7 +2138,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>18</v>
       </c>
@@ -2153,7 +2161,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>6</v>
       </c>
@@ -2176,7 +2184,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>6</v>
       </c>
@@ -2199,7 +2207,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>6</v>
       </c>
@@ -2222,7 +2230,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -2245,7 +2253,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -2268,7 +2276,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -2291,7 +2299,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="s">
         <v>10</v>
@@ -2302,7 +2310,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>13</v>
       </c>
@@ -2325,7 +2333,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>24</v>
       </c>
@@ -2348,7 +2356,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>2</v>
       </c>
@@ -2371,7 +2379,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>8</v>
       </c>
@@ -2394,7 +2402,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>8</v>
       </c>
@@ -2417,7 +2425,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>8</v>
       </c>
@@ -2440,7 +2448,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>8</v>
       </c>
@@ -2463,7 +2471,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>4</v>
       </c>
@@ -2486,7 +2494,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>1</v>
       </c>
@@ -2509,7 +2517,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>1</v>
       </c>
@@ -2532,7 +2540,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>1</v>
       </c>
@@ -2555,7 +2563,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2564,12 +2572,12 @@
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
     </row>
-    <row r="56" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B56" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>13</v>
       </c>
@@ -2589,7 +2597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>2</v>
       </c>
@@ -2609,7 +2617,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>2</v>
       </c>
@@ -2629,7 +2637,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>2</v>
       </c>
@@ -2652,7 +2660,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>2</v>
       </c>
@@ -2675,7 +2683,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>1</v>
       </c>
@@ -2698,7 +2706,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>1</v>
       </c>
@@ -2721,7 +2729,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>1</v>
       </c>
@@ -2744,7 +2752,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>1</v>
       </c>
@@ -2766,8 +2774,11 @@
       <c r="G65" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H65" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>3</v>
       </c>
@@ -2789,8 +2800,11 @@
       <c r="G66" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H66" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>1</v>
       </c>
@@ -2813,7 +2827,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>2</v>
       </c>
@@ -2839,7 +2853,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>1</v>
       </c>
@@ -2862,7 +2876,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>1</v>
       </c>
@@ -2885,7 +2899,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>1</v>
       </c>
@@ -2908,7 +2922,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>1</v>
       </c>
@@ -2931,7 +2945,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>1</v>
       </c>
@@ -2954,7 +2968,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>1</v>
       </c>
@@ -2977,7 +2991,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>1</v>
       </c>
@@ -3000,7 +3014,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="5"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
@@ -3009,12 +3023,12 @@
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
     </row>
-    <row r="77" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B77" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>13</v>
       </c>
@@ -3034,7 +3048,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>8</v>
       </c>
@@ -3054,7 +3068,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>8</v>
       </c>
@@ -3074,7 +3088,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>4</v>
       </c>
@@ -3097,7 +3111,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>2</v>
       </c>
@@ -3120,7 +3134,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>2</v>
       </c>
@@ -3143,7 +3157,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>6</v>
       </c>
@@ -3166,7 +3180,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>4</v>
       </c>
@@ -3189,7 +3203,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>2</v>
       </c>
@@ -3212,7 +3226,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>1</v>
       </c>
@@ -3235,7 +3249,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>1</v>
       </c>
@@ -3258,7 +3272,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>1</v>
       </c>
@@ -3281,7 +3295,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>2</v>
       </c>
@@ -3304,7 +3318,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>2</v>
       </c>
@@ -3327,7 +3341,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="5"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -3336,13 +3350,13 @@
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A93" s="3"/>
       <c r="B93" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>13</v>
       </c>
@@ -3362,7 +3376,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>5</v>
       </c>
@@ -3382,7 +3396,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>2</v>
       </c>
@@ -3402,7 +3416,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>1</v>
       </c>
@@ -3425,7 +3439,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>4</v>
       </c>
@@ -3448,7 +3462,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>17</v>
       </c>
@@ -3471,7 +3485,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>15</v>
       </c>
@@ -3494,7 +3508,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>4</v>
       </c>
@@ -3517,7 +3531,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>2</v>
       </c>
@@ -3540,7 +3554,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>1</v>
       </c>
@@ -3563,7 +3577,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>1</v>
       </c>
@@ -3586,7 +3600,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>2</v>
       </c>
@@ -3609,7 +3623,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>7</v>
       </c>
@@ -3632,7 +3646,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>3</v>
       </c>
@@ -3655,7 +3669,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>3</v>
       </c>
@@ -3678,7 +3692,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>2</v>
       </c>
@@ -3701,7 +3715,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>2</v>
       </c>
@@ -3724,7 +3738,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>2</v>
       </c>
@@ -3747,7 +3761,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>1</v>
       </c>
@@ -3770,7 +3784,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>

</xml_diff>